<commit_message>
Soon repository will be opened
</commit_message>
<xml_diff>
--- a/Функционал.xlsx
+++ b/Функционал.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
   <si>
     <t xml:space="preserve">Таблица всех функций бота</t>
   </si>
@@ -218,6 +218,9 @@
     <t xml:space="preserve">ExcelWriter</t>
   </si>
   <si>
+    <t xml:space="preserve">FinanceBot</t>
+  </si>
+  <si>
     <t xml:space="preserve">Название функции</t>
   </si>
   <si>
@@ -227,6 +230,12 @@
     <t xml:space="preserve">FinanceBot.c</t>
   </si>
   <si>
+    <t xml:space="preserve">getHelpMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getHelp</t>
+  </si>
+  <si>
     <t xml:space="preserve">rowsCount</t>
   </si>
   <si>
@@ -242,6 +251,9 @@
     <t xml:space="preserve">writeColumnNames</t>
   </si>
   <si>
+    <t xml:space="preserve">productSold</t>
+  </si>
+  <si>
     <t xml:space="preserve">getFieldsAverageSum</t>
   </si>
   <si>
@@ -254,6 +266,9 @@
     <t xml:space="preserve">generateExcelFile</t>
   </si>
   <si>
+    <t xml:space="preserve">getReplyFromDatabase</t>
+  </si>
+  <si>
     <t xml:space="preserve">fieldsAreNotSQLCommands</t>
   </si>
   <si>
@@ -264,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">getFilePath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isValidFunction</t>
   </si>
   <si>
     <t xml:space="preserve">getFieldsSum</t>
@@ -355,6 +373,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -377,12 +396,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -448,7 +469,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -509,6 +530,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -525,10 +550,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -543,10 +564,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -637,8 +654,8 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,10 +948,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -947,6 +964,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,303 +988,329 @@
         <v>64</v>
       </c>
       <c r="K1" s="13"/>
+      <c r="M1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
       <c r="G2" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14"/>
       <c r="J2" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K2" s="13"/>
+      <c r="M2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>70</v>
+      <c r="A4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="17" t="s">
-        <v>71</v>
+      <c r="G4" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="17" t="s">
-        <v>72</v>
+      <c r="J4" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="17" t="s">
-        <v>75</v>
+      <c r="G5" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="17" t="s">
-        <v>76</v>
+      <c r="J5" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="17" t="s">
-        <v>79</v>
+      <c r="G6" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="17" t="s">
-        <v>80</v>
+      <c r="J6" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>80</v>
+        <v>85</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>82</v>
+      <c r="A7" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="17" t="s">
-        <v>83</v>
+      <c r="G7" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I7" s="14"/>
+      <c r="N7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>85</v>
+      <c r="A8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="17" t="s">
-        <v>86</v>
+      <c r="G8" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="I8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>89</v>
+      <c r="A9" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="17" t="s">
-        <v>90</v>
+      <c r="G9" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="I9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>93</v>
+      <c r="A10" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>99</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="17" t="s">
-        <v>95</v>
+      <c r="G10" s="18" t="s">
+        <v>101</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>97</v>
+      <c r="A11" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>103</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="17" t="s">
-        <v>98</v>
+      <c r="G11" s="18" t="s">
+        <v>104</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>100</v>
+      <c r="A12" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>106</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="17" t="s">
-        <v>101</v>
+      <c r="G12" s="18" t="s">
+        <v>107</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>103</v>
+      <c r="A13" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>109</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="26"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>104</v>
+      <c r="D14" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="26"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>105</v>
+      <c r="D15" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>111</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="26"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="14"/>
@@ -1275,11 +1320,12 @@
       <c r="H16" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>

</xml_diff>